<commit_message>
rename and update files
</commit_message>
<xml_diff>
--- a/lendingrisk/features.xlsx
+++ b/lendingrisk/features.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1BA487-7ED4-4039-A167-41E05767BB82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE5AF99-DCC4-4730-A57E-F0627C21D836}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="features" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="475">
   <si>
     <t>column</t>
   </si>
@@ -1490,6 +1490,11 @@
   </si>
   <si>
     <t>均编码+重要特征分组求max mean等</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同上，但是删除
+importance=0的特征</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2741,8 +2746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F2285A-0580-4E4D-8803-3C6614005D3B}">
   <dimension ref="A1:S351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J202" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -7945,8 +7950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C19AEF-B212-42A2-B6A6-9D7BF18D40F8}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E10:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -8152,19 +8157,35 @@
         <v>0.74002585508304697</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="22.8">
+    <row r="8" spans="1:13" ht="45.6">
       <c r="A8" s="19"/>
       <c r="B8" s="27"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
+      <c r="C8" s="16" t="s">
+        <v>474</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>159</v>
+      </c>
       <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
+      <c r="I8" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>161</v>
+      </c>
       <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
+      <c r="L8" s="29">
+        <v>0.74001145813677704</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="22.8">
       <c r="A9" s="19"/>

</xml_diff>